<commit_message>
Naprawione edytowanie opcji zapytań.
</commit_message>
<xml_diff>
--- a/Lang TODO.xlsx
+++ b/Lang TODO.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
   <si>
     <t>prawidłowe odpowiedzi - np. dla (to )want powinno robić dwie opcje: to want / want</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Przestawić, że [Weight] może być 0</t>
+  </si>
+  <si>
+    <t>Jeżeli dla danego pytania nie ma ani jednego QueryOptions z [Displayed] = True, wtedy ma wybierać spośród pozostałych.</t>
   </si>
 </sst>
 </file>
@@ -170,49 +173,7 @@
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -531,9 +492,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -701,7 +664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="38.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -789,8 +752,19 @@
         <v>0</v>
       </c>
     </row>
+    <row r="15" spans="1:6" ht="25.5">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:F14">
+  <conditionalFormatting sqref="A2:F17">
     <cfRule type="expression" dxfId="3" priority="5">
       <formula>IF($F2=1,1,0)</formula>
     </cfRule>
@@ -807,7 +781,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F10:F14">
+  <conditionalFormatting sqref="F10:F17">
     <cfRule type="iconSet" priority="10">
       <iconSet iconSet="3Symbols" showValue="0">
         <cfvo type="percent" val="0"/>

</xml_diff>

<commit_message>
1) Zmieniona logika do wyliczania ile powtórzeń danego zapytania powinny być w danej sesji testowej. 2) Naprawiony błąd, który pojawiał się po zakończeniu sesji. 3) Zapisywanie wyników sesji w bazie danych.
</commit_message>
<xml_diff>
--- a/Lang TODO.xlsx
+++ b/Lang TODO.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Arkusz3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -173,21 +174,7 @@
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -495,7 +482,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -678,7 +665,7 @@
         <v>15</v>
       </c>
       <c r="F10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -765,10 +752,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:F17">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="1" priority="5">
       <formula>IF($F2=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="0" priority="6">
       <formula>IF($F2&lt;&gt;1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>